<commit_message>
make more time for sleep
</commit_message>
<xml_diff>
--- a/result/backup-data/back-up0.xlsx
+++ b/result/backup-data/back-up0.xlsx
@@ -634,19 +634,19 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FC충주</t>
+          <t>FC안양</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>창단일자
-20180101
-주소
-충북 충주시 대림로 85 (호암동, 충주종합운동장) 3번게이트내 FC충주
-연락처
-043-848-7755
-감독
-김종필
+20130202
+주소
+경기도 안양시 동안구 평촌대로 389 (비산동, 안양종합운동장) 안양종합운동장 내 FC안양 사무국
+연락처
+031-476-3500
+감독
+이우형
 팀 관리에서 팀 SNS를 등록하세요</t>
         </is>
       </c>

</xml_diff>

<commit_message>
have to fix run.py
</commit_message>
<xml_diff>
--- a/result/backup-data/back-up0.xlsx
+++ b/result/backup-data/back-up0.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -680,19 +680,520 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>강원고성군간성클럽</t>
+          <t>강원고성군거진FC</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
           <t>창단일자
-20140302
-주소
-강원 고성군 간성읍 수성로 111 (상리, 종합운동장)
-연락처
-010-2171-6033
-감독
-박득쇠
+20210101
+주소
+강원도 고성군 거진읍 거진운동장길 30 (거진리) 1
+연락처
+010-4677-7077
+감독
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>강원고성군고성사랑축구회</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>창단일자
+20180102
+주소
+강원 고성군 토성면 장새미1길 11 (용암리) 용암리
+연락처
+010-2828-4338
+감독
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>강원고성군달홀FC</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>창단일자
+20110101
+주소
+강원 고성군 간성읍 간성로 64 정일빌딩 3층
+연락처
+010-7708-4342
+감독
+최서희
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>강원고성군죽왕축구회</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>창단일자
+20050101
+주소
+강원도 고성군 간성읍 탑동길 12 (신안리, 고성경찰서) 금강파출소
+연락처
+010-9300-5682
+감독
+강완식
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>강원고성군토요축구회</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>창단일자
+1974
+주소
+강원 고성군 거진읍 화포2길 26 (화포리)
+연락처
+010-8727-2188
+감독
+고경태
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>강원동해시초록생활축구회</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>창단일자
+19780120
+주소
+강원 동해시 중앙로 143 (천곡동, 행복드림아파트) 105동 803호
+연락처
+010-5574-0690
+감독
+심영철
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>강원동해시해일생활축구회</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>창단일자
+19990101
+주소
+강원도 동해시 효자남길 26-1 (동회동, 동보상가) 꿀꿀이뱃살
+연락처
+010-9728-0717
+감독
+배기표
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>강원삼척시FC이글스</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>창단일자
+20000101
+주소
+강원도 삼척시 동해대로 4234 (교동, 삼척종합운동장) 삼척시축구협회
+연락처
+010-6375-1414
+감독
+지중근
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>강원삼척시가람FC</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>창단일자
+20200501
+주소
+강원 삼척시 중앙로4길 14-34 가온누리스포츠
+연락처
+010-7188-0104
+감독
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>강원삼척시라온FC</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>창단일자
+20200129
+주소
+강원 삼척시 동해대로 4234 (교동, 삼척종합운동장)
+연락처
+010-6876-7720
+감독
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>강원삼척시미리내FC</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>창단일자
+20230102
+주소
+강원 삼척시 도계읍 장원길 63 (도계리, 경동아파트) 12동 307호
+연락처
+010-4614-1984
+감독
+김동진
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>강원삼척시삼척동자FC</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>창단일자
+20220711
+주소
+강원 삼척시 중앙시장1길 22-23 (남양동, 세연상가아파트) 708호
+연락처
+010-9528-2260
+감독
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>강원삼척시미리내FC</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>창단일자
+20230102
+주소
+강원 삼척시 도계읍 장원길 63 (도계리, 경동아파트) 12동 307호
+연락처
+010-4614-1984
+감독
+김동진
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>강원삼척시원더플FC</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>창단일자
+20161002
+주소
+강원 삼척시 동해대로 4234 (교동, 삼척종합운동장) 삼척시축구협회
+연락처
+010-2758-1516
+감독
+이광철
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>강원속초시일오축구회</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>창단일자
+19810813
+주소
+강원도 속초시 번영로129번길 25 (동명동) (동명동)
+연락처
+010-4370-6085
+감독
+김명수
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>강원속초시청해FC축구회</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>창단일자
+20180701
+주소
+강원 속초시 중앙로 96 (청학동) 로데오센터빌딩 4층
+연락처
+010-2803-1271
+감독
+박일균
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>강원속초시클래스</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>창단일자
+20160101
+주소
+강원 속초시 청대마을길 37 (조양동) 청대리막국수
+연락처
+010-3699-5210
+감독
+장유민
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>강원속초시한솔축구회</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>창단일자
+2001
+주소
+강원 속초시 청대마을길 16-1 (조양동)신태용 축구교실 속초센터
+연락처
+010-5389-9489
+감독
+이서호
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>강원속초시해마축구회</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>창단일자
+19990301
+주소
+강원도 속초시 청대로204번길 40 (조양동, 부영아파트5단지) 501동~508동 505동111호
+연락처
+010-3115-4285
+감독
+김병일
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>강원속초시현대축구회</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>창단일자
+19890101
+주소
+강원도 속초시 소평로 68 (조양동) 257-4
+연락처
+010-5362-7747
+감독
+김성백
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>강원양구군BAEKDUUTD</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>창단일자
+20211118
+주소
+강원 양구군 동면 금강산로 1801 (임당리, 대암아파트) e동 402호
+연락처
+010-2004-7995
+감독
+강민재
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>강원속초시현대축구회</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>창단일자
+19890101
+주소
+강원도 속초시 소평로 68 (조양동) 257-4
+연락처
+010-5362-7747
+감독
+김성백
+팀 관리에서 팀 SNS를 등록하세요</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>강원영월군동강FC60대</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>창단일자
+20000301
+주소
+강원도 영월군 영월읍 제방안길 100 (하송리, 영월스포츠파크) 영월군체육회
+연락처
+010-5214-2290
+감독
+방극원1
 팀 관리에서 팀 SNS를 등록하세요</t>
         </is>
       </c>

</xml_diff>